<commit_message>
Updates to data, MFQ fix, and Graph creation
</commit_message>
<xml_diff>
--- a/ProcessSimulator/N=10 Graphs.xlsx
+++ b/ProcessSimulator/N=10 Graphs.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\MST\Fall 2020\CS 3800\Project\Simulator\Process-Memory-Mangaement-Simulation\ProcessSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF21B75-B102-4669-82DE-C391F1EF7515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80C7477-824E-4AFD-BA0C-F278386A0C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="5">
   <si>
     <t>Input</t>
   </si>
@@ -37,6 +45,9 @@
   </si>
   <si>
     <t>Runtime</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -2654,307 +2665,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>885</c:v>
+                  <c:v>417</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>915</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>899</c:v>
+                  <c:v>378</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>940</c:v>
+                  <c:v>403</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>901</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5564</c:v>
+                  <c:v>467</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>920</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>924</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1201</c:v>
+                  <c:v>394</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>928</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1212</c:v>
+                  <c:v>722</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>873</c:v>
+                  <c:v>436</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>824</c:v>
+                  <c:v>394</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>882</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>734</c:v>
+                  <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1139</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>873</c:v>
+                  <c:v>426</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>962</c:v>
+                  <c:v>446</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1167</c:v>
+                  <c:v>545</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1071</c:v>
+                  <c:v>436</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17209</c:v>
+                  <c:v>362</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>799</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>932</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1024</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>906</c:v>
+                  <c:v>447</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>922</c:v>
+                  <c:v>659</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>724</c:v>
+                  <c:v>536</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>933</c:v>
+                  <c:v>516</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>837</c:v>
+                  <c:v>468</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>903</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1086</c:v>
+                  <c:v>479</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>16369</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1120</c:v>
+                  <c:v>593</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>687</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>941</c:v>
+                  <c:v>633</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1079</c:v>
+                  <c:v>4831</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>781</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>924</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1289</c:v>
+                  <c:v>372</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>897</c:v>
+                  <c:v>581</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10673</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>924</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1022</c:v>
+                  <c:v>448</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1075</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>895</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>783</c:v>
+                  <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>802</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>913</c:v>
+                  <c:v>537</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1602</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1047</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>23222</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1248</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>887</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1080</c:v>
+                  <c:v>1537</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>781</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>949</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2916</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>17779</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>966</c:v>
+                  <c:v>369</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>870</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1034</c:v>
+                  <c:v>477</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>876</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>934</c:v>
+                  <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>849</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>807</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1180</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>15737</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1348</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>757</c:v>
+                  <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1377</c:v>
+                  <c:v>412</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>801</c:v>
+                  <c:v>347</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1502</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>909</c:v>
+                  <c:v>368</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1113</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>11664</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5114</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>941</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1177</c:v>
+                  <c:v>388</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1190</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1022</c:v>
+                  <c:v>743</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1444</c:v>
+                  <c:v>403</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>586</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1448</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>823</c:v>
+                  <c:v>649</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1285</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>20014</c:v>
+                  <c:v>443</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1682</c:v>
+                  <c:v>737</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1160</c:v>
+                  <c:v>448</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>951</c:v>
+                  <c:v>232</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1456</c:v>
+                  <c:v>423</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1014</c:v>
+                  <c:v>252</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1518</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>919</c:v>
+                  <c:v>434</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1459</c:v>
+                  <c:v>566</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1827</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1637</c:v>
+                  <c:v>457</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>3045</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1473</c:v>
+                  <c:v>299</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1459</c:v>
+                  <c:v>443</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1827</c:v>
+                  <c:v>737</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1637</c:v>
+                  <c:v>448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5846,307 +5857,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>5.2103999999999999</c:v>
+                  <c:v>5.1963900000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5740800000000004</c:v>
+                  <c:v>6.05044</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3038299999999996</c:v>
+                  <c:v>6.3765900000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.8690999999999995</c:v>
+                  <c:v>6.92333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.9435</c:v>
+                  <c:v>8.0909499999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2181199999999999</c:v>
+                  <c:v>4.6902400000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4044999999999996</c:v>
+                  <c:v>5.6147200000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.9194200000000006</c:v>
+                  <c:v>6.6326200000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.9818300000000004</c:v>
+                  <c:v>7.5321400000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.7611800000000004</c:v>
+                  <c:v>5.6950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5917300000000001</c:v>
+                  <c:v>5.9410699999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.1599300000000001</c:v>
+                  <c:v>5.2497600000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.0221400000000003</c:v>
+                  <c:v>6.1201600000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.8157699999999997</c:v>
+                  <c:v>6.6916700000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.943300000000001</c:v>
+                  <c:v>10.5783</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.0999</c:v>
+                  <c:v>9.9502799999999993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1205299999999996</c:v>
+                  <c:v>4.9667500000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.9841200000000008</c:v>
+                  <c:v>8.1537299999999995</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.8613600000000003</c:v>
+                  <c:v>7.3478199999999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9366699999999994</c:v>
+                  <c:v>8.0571800000000007</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.0462199999999999</c:v>
+                  <c:v>9.0684500000000003</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.0438400000000003</c:v>
+                  <c:v>6.5860700000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.6637000000000004</c:v>
+                  <c:v>7.0331000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.9209</c:v>
+                  <c:v>10.450799999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10.6959</c:v>
+                  <c:v>8.3434500000000007</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.4982600000000001</c:v>
+                  <c:v>5.26607</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.3892500000000005</c:v>
+                  <c:v>7.95444</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.4681199999999999</c:v>
+                  <c:v>6.4983300000000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.3136200000000002</c:v>
+                  <c:v>5.0869799999999996</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10.7112</c:v>
+                  <c:v>7.8616700000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.3423299999999996</c:v>
+                  <c:v>6.8992899999999997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11.910600000000001</c:v>
+                  <c:v>10.061199999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.0297099999999997</c:v>
+                  <c:v>6.50115</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.4463600000000003</c:v>
+                  <c:v>6.7602799999999998</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.1614399999999998</c:v>
+                  <c:v>5.0650000000000004</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.6725199999999996</c:v>
+                  <c:v>6.085</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>7.0993599999999999</c:v>
+                  <c:v>5.7175399999999996</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.0715</c:v>
+                  <c:v>9.6199999999999992</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.3982799999999997</c:v>
+                  <c:v>7.6003999999999996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.9726800000000004</c:v>
+                  <c:v>5.4971800000000002</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9.6755099999999992</c:v>
+                  <c:v>9.0327800000000007</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.3610600000000002</c:v>
+                  <c:v>4.2816700000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.2281300000000002</c:v>
+                  <c:v>5.6983300000000003</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.8568899999999999</c:v>
+                  <c:v>7.4517499999999997</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.9162699999999999</c:v>
+                  <c:v>6.2011900000000004</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.4484500000000002</c:v>
+                  <c:v>4.5525399999999996</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.9976900000000004</c:v>
+                  <c:v>8.8083299999999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.8617499999999998</c:v>
+                  <c:v>4.9010699999999998</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>11.195600000000001</c:v>
+                  <c:v>9.4648400000000006</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.7292800000000002</c:v>
+                  <c:v>5.8238099999999999</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>8.6945499999999996</c:v>
+                  <c:v>5.9154799999999996</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8.5318699999999996</c:v>
+                  <c:v>6.7175000000000002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.2790100000000004</c:v>
+                  <c:v>4.8410700000000002</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6.0329100000000002</c:v>
+                  <c:v>5.3291700000000004</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>8.2269600000000001</c:v>
+                  <c:v>8.0314300000000003</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>11.7538</c:v>
+                  <c:v>9.3491700000000009</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>12.1038</c:v>
+                  <c:v>9.2057500000000001</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7.4957500000000001</c:v>
+                  <c:v>5.6694399999999998</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>9.6051900000000003</c:v>
+                  <c:v>8.5897199999999998</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.5372899999999996</c:v>
+                  <c:v>5.9082499999999998</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>7.0077800000000003</c:v>
+                  <c:v>5.9469399999999997</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>9.7489000000000008</c:v>
+                  <c:v>6.5666700000000002</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>6.2360699999999998</c:v>
+                  <c:v>4.9028999999999998</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>7.9900700000000002</c:v>
+                  <c:v>5.1776200000000001</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>9.9858799999999999</c:v>
+                  <c:v>4.2708300000000001</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>11.2415</c:v>
+                  <c:v>7.7083300000000001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>8.5413899999999998</c:v>
+                  <c:v>6.8635700000000002</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>10.5395</c:v>
+                  <c:v>6.75143</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>10.7964</c:v>
+                  <c:v>5.6183300000000003</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6.3501899999999996</c:v>
+                  <c:v>5.7698799999999997</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>8.9309399999999997</c:v>
+                  <c:v>4.9414300000000004</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6.2254800000000001</c:v>
+                  <c:v>6.9955600000000002</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>8.8520000000000003</c:v>
+                  <c:v>9.4279799999999998</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>11.0463</c:v>
+                  <c:v>6.2187299999999999</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>6.9434800000000001</c:v>
+                  <c:v>5.9084099999999999</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>7.4385399999999997</c:v>
+                  <c:v>5.7540500000000003</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>6.3161800000000001</c:v>
+                  <c:v>5.4641700000000002</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>7.2251099999999999</c:v>
+                  <c:v>5.3377800000000004</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>7.5076799999999997</c:v>
+                  <c:v>8.0648800000000005</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>7.6157700000000004</c:v>
+                  <c:v>5.6943700000000002</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>7.5739099999999997</c:v>
+                  <c:v>6.6560300000000003</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>8.6494700000000009</c:v>
+                  <c:v>4.3283300000000002</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>5.1710599999999998</c:v>
+                  <c:v>4.9192099999999996</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>7.2497499999999997</c:v>
+                  <c:v>5.9096000000000002</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>7.8109999999999999</c:v>
+                  <c:v>6.4541700000000004</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>6.5839800000000004</c:v>
+                  <c:v>4.3748800000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>7.0901100000000001</c:v>
+                  <c:v>5.4055999999999997</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4.5538400000000001</c:v>
+                  <c:v>5.7472200000000004</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>8.4394899999999993</c:v>
+                  <c:v>4.4325000000000001</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>6.1083400000000001</c:v>
+                  <c:v>8.1281700000000008</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>7.7574800000000002</c:v>
+                  <c:v>6.36972</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>8.9840900000000001</c:v>
+                  <c:v>8.0448400000000007</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>10.0192</c:v>
+                  <c:v>5.9371</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>7.8626399999999999</c:v>
+                  <c:v>7.4776199999999999</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>6.6682800000000002</c:v>
+                  <c:v>5.7110300000000001</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>7.9331300000000002</c:v>
+                  <c:v>6.28024</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>6.8227900000000004</c:v>
+                  <c:v>9.0514299999999999</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>10.9648</c:v>
+                  <c:v>4.7957099999999997</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>7.8626399999999999</c:v>
+                  <c:v>4.3748800000000001</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>6.6682800000000002</c:v>
+                  <c:v>5.4055999999999997</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.9331300000000002</c:v>
+                  <c:v>5.7472200000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7572,13 +7583,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7608,13 +7619,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7908,10 +7919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM102"/>
+  <dimension ref="A1:AM103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="Y168" sqref="Y168"/>
+    <sheetView tabSelected="1" topLeftCell="L58" workbookViewId="0">
+      <selection activeCell="AM103" sqref="AM103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8103,13 +8114,13 @@
         <v>8</v>
       </c>
       <c r="AK2">
-        <v>78</v>
+        <v>31.2</v>
       </c>
       <c r="AL2">
-        <v>5.2103999999999999</v>
+        <v>5.1963900000000001</v>
       </c>
       <c r="AM2">
-        <v>885</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
@@ -8201,13 +8212,13 @@
         <v>8</v>
       </c>
       <c r="AK3">
-        <v>66.7</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="AL3">
-        <v>7.5740800000000004</v>
+        <v>6.05044</v>
       </c>
       <c r="AM3">
-        <v>915</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -8299,13 +8310,13 @@
         <v>8</v>
       </c>
       <c r="AK4">
-        <v>84.2</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="AL4">
-        <v>6.3038299999999996</v>
+        <v>6.3765900000000002</v>
       </c>
       <c r="AM4">
-        <v>899</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
@@ -8397,13 +8408,13 @@
         <v>8</v>
       </c>
       <c r="AK5">
-        <v>78.599999999999994</v>
+        <v>33.6</v>
       </c>
       <c r="AL5">
-        <v>9.8690999999999995</v>
+        <v>6.92333</v>
       </c>
       <c r="AM5">
-        <v>940</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
@@ -8495,13 +8506,13 @@
         <v>8</v>
       </c>
       <c r="AK6">
-        <v>80.3</v>
+        <v>26.7</v>
       </c>
       <c r="AL6">
-        <v>10.9435</v>
+        <v>8.0909499999999994</v>
       </c>
       <c r="AM6">
-        <v>901</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -8593,13 +8604,13 @@
         <v>8</v>
       </c>
       <c r="AK7">
-        <v>72.900000000000006</v>
+        <v>28.5</v>
       </c>
       <c r="AL7">
-        <v>6.2181199999999999</v>
+        <v>4.6902400000000002</v>
       </c>
       <c r="AM7">
-        <v>5564</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -8691,13 +8702,13 @@
         <v>8</v>
       </c>
       <c r="AK8">
-        <v>83.6</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="AL8">
-        <v>7.4044999999999996</v>
+        <v>5.6147200000000002</v>
       </c>
       <c r="AM8">
-        <v>920</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
@@ -8789,13 +8800,13 @@
         <v>8</v>
       </c>
       <c r="AK9">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="AL9">
-        <v>8.9194200000000006</v>
+        <v>6.6326200000000002</v>
       </c>
       <c r="AM9">
-        <v>924</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
@@ -8887,13 +8898,13 @@
         <v>8</v>
       </c>
       <c r="AK10">
-        <v>63.3</v>
+        <v>21.9</v>
       </c>
       <c r="AL10">
-        <v>9.9818300000000004</v>
+        <v>7.5321400000000001</v>
       </c>
       <c r="AM10">
-        <v>1201</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
@@ -8985,13 +8996,13 @@
         <v>8</v>
       </c>
       <c r="AK11">
-        <v>55</v>
+        <v>22.4</v>
       </c>
       <c r="AL11">
-        <v>5.7611800000000004</v>
+        <v>5.6950000000000003</v>
       </c>
       <c r="AM11">
-        <v>928</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
@@ -9083,13 +9094,13 @@
         <v>8</v>
       </c>
       <c r="AK12">
-        <v>78.2</v>
+        <v>45</v>
       </c>
       <c r="AL12">
-        <v>5.5917300000000001</v>
+        <v>5.9410699999999999</v>
       </c>
       <c r="AM12">
-        <v>1212</v>
+        <v>722</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
@@ -9181,13 +9192,13 @@
         <v>8</v>
       </c>
       <c r="AK13">
-        <v>68.5</v>
+        <v>33.1</v>
       </c>
       <c r="AL13">
-        <v>6.1599300000000001</v>
+        <v>5.2497600000000002</v>
       </c>
       <c r="AM13">
-        <v>873</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
@@ -9279,13 +9290,13 @@
         <v>8</v>
       </c>
       <c r="AK14">
-        <v>80.8</v>
+        <v>33.9</v>
       </c>
       <c r="AL14">
-        <v>8.0221400000000003</v>
+        <v>6.1201600000000003</v>
       </c>
       <c r="AM14">
-        <v>824</v>
+        <v>394</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
@@ -9377,13 +9388,13 @@
         <v>8</v>
       </c>
       <c r="AK15">
-        <v>68.8</v>
+        <v>29.1</v>
       </c>
       <c r="AL15">
-        <v>7.8157699999999997</v>
+        <v>6.6916700000000002</v>
       </c>
       <c r="AM15">
-        <v>882</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
@@ -9475,13 +9486,13 @@
         <v>8</v>
       </c>
       <c r="AK16">
-        <v>68.400000000000006</v>
+        <v>37.1</v>
       </c>
       <c r="AL16">
-        <v>12.943300000000001</v>
+        <v>10.5783</v>
       </c>
       <c r="AM16">
-        <v>734</v>
+        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
@@ -9573,13 +9584,13 @@
         <v>8</v>
       </c>
       <c r="AK17">
-        <v>70.599999999999994</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="AL17">
-        <v>10.0999</v>
+        <v>9.9502799999999993</v>
       </c>
       <c r="AM17">
-        <v>1139</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
@@ -9671,13 +9682,13 @@
         <v>8</v>
       </c>
       <c r="AK18">
-        <v>90.3</v>
+        <v>30.6</v>
       </c>
       <c r="AL18">
-        <v>6.1205299999999996</v>
+        <v>4.9667500000000002</v>
       </c>
       <c r="AM18">
-        <v>873</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
@@ -9769,13 +9780,13 @@
         <v>8</v>
       </c>
       <c r="AK19">
-        <v>85.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="AL19">
-        <v>9.9841200000000008</v>
+        <v>8.1537299999999995</v>
       </c>
       <c r="AM19">
-        <v>962</v>
+        <v>446</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
@@ -9867,13 +9878,13 @@
         <v>8</v>
       </c>
       <c r="AK20">
-        <v>95.9</v>
+        <v>48.9</v>
       </c>
       <c r="AL20">
-        <v>6.8613600000000003</v>
+        <v>7.3478199999999996</v>
       </c>
       <c r="AM20">
-        <v>1167</v>
+        <v>545</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
@@ -9965,13 +9976,13 @@
         <v>8</v>
       </c>
       <c r="AK21">
-        <v>104.5</v>
+        <v>48.3</v>
       </c>
       <c r="AL21">
-        <v>8.9366699999999994</v>
+        <v>8.0571800000000007</v>
       </c>
       <c r="AM21">
-        <v>1071</v>
+        <v>436</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
@@ -10063,13 +10074,13 @@
         <v>8</v>
       </c>
       <c r="AK22">
-        <v>88.8</v>
+        <v>33.1</v>
       </c>
       <c r="AL22">
-        <v>8.0462199999999999</v>
+        <v>9.0684500000000003</v>
       </c>
       <c r="AM22">
-        <v>17209</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
@@ -10161,13 +10172,13 @@
         <v>8</v>
       </c>
       <c r="AK23">
-        <v>50.5</v>
+        <v>23.3</v>
       </c>
       <c r="AL23">
-        <v>7.0438400000000003</v>
+        <v>6.5860700000000003</v>
       </c>
       <c r="AM23">
-        <v>799</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
@@ -10259,13 +10270,13 @@
         <v>8</v>
       </c>
       <c r="AK24">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="AL24">
-        <v>7.6637000000000004</v>
+        <v>7.0331000000000001</v>
       </c>
       <c r="AM24">
-        <v>932</v>
+        <v>520</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
@@ -10357,13 +10368,13 @@
         <v>8</v>
       </c>
       <c r="AK25">
-        <v>75.8</v>
+        <v>29.5</v>
       </c>
       <c r="AL25">
-        <v>13.9209</v>
+        <v>10.450799999999999</v>
       </c>
       <c r="AM25">
-        <v>1024</v>
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
@@ -10455,13 +10466,13 @@
         <v>8</v>
       </c>
       <c r="AK26">
-        <v>77.900000000000006</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="AL26">
-        <v>10.6959</v>
+        <v>8.3434500000000007</v>
       </c>
       <c r="AM26">
-        <v>906</v>
+        <v>447</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
@@ -10553,13 +10564,13 @@
         <v>8</v>
       </c>
       <c r="AK27">
-        <v>79.599999999999994</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="AL27">
-        <v>5.4982600000000001</v>
+        <v>5.26607</v>
       </c>
       <c r="AM27">
-        <v>922</v>
+        <v>659</v>
       </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
@@ -10651,13 +10662,13 @@
         <v>8</v>
       </c>
       <c r="AK28">
-        <v>64.400000000000006</v>
+        <v>24.9</v>
       </c>
       <c r="AL28">
-        <v>8.3892500000000005</v>
+        <v>7.95444</v>
       </c>
       <c r="AM28">
-        <v>724</v>
+        <v>536</v>
       </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
@@ -10749,13 +10760,13 @@
         <v>8</v>
       </c>
       <c r="AK29">
-        <v>99.5</v>
+        <v>53.8</v>
       </c>
       <c r="AL29">
-        <v>6.4681199999999999</v>
+        <v>6.4983300000000002</v>
       </c>
       <c r="AM29">
-        <v>933</v>
+        <v>516</v>
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
@@ -10847,13 +10858,13 @@
         <v>8</v>
       </c>
       <c r="AK30">
-        <v>66.599999999999994</v>
+        <v>28.1</v>
       </c>
       <c r="AL30">
-        <v>6.3136200000000002</v>
+        <v>5.0869799999999996</v>
       </c>
       <c r="AM30">
-        <v>837</v>
+        <v>468</v>
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
@@ -10945,13 +10956,13 @@
         <v>8</v>
       </c>
       <c r="AK31">
-        <v>60</v>
+        <v>22.7</v>
       </c>
       <c r="AL31">
-        <v>10.7112</v>
+        <v>7.8616700000000002</v>
       </c>
       <c r="AM31">
-        <v>903</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
@@ -11043,13 +11054,13 @@
         <v>8</v>
       </c>
       <c r="AK32">
-        <v>67.599999999999994</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="AL32">
-        <v>7.3423299999999996</v>
+        <v>6.8992899999999997</v>
       </c>
       <c r="AM32">
-        <v>1086</v>
+        <v>479</v>
       </c>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
@@ -11141,13 +11152,13 @@
         <v>8</v>
       </c>
       <c r="AK33">
-        <v>58.4</v>
+        <v>32.1</v>
       </c>
       <c r="AL33">
-        <v>11.910600000000001</v>
+        <v>10.061199999999999</v>
       </c>
       <c r="AM33">
-        <v>16369</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
@@ -11239,13 +11250,13 @@
         <v>8</v>
       </c>
       <c r="AK34">
-        <v>94.4</v>
+        <v>49.8</v>
       </c>
       <c r="AL34">
-        <v>8.0297099999999997</v>
+        <v>6.50115</v>
       </c>
       <c r="AM34">
-        <v>1120</v>
+        <v>593</v>
       </c>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
@@ -11337,13 +11348,13 @@
         <v>8</v>
       </c>
       <c r="AK35">
-        <v>72.5</v>
+        <v>27.9</v>
       </c>
       <c r="AL35">
-        <v>7.4463600000000003</v>
+        <v>6.7602799999999998</v>
       </c>
       <c r="AM35">
-        <v>687</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
@@ -11435,13 +11446,13 @@
         <v>8</v>
       </c>
       <c r="AK36">
-        <v>47.1</v>
+        <v>22.8</v>
       </c>
       <c r="AL36">
-        <v>6.1614399999999998</v>
+        <v>5.0650000000000004</v>
       </c>
       <c r="AM36">
-        <v>941</v>
+        <v>633</v>
       </c>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
@@ -11533,13 +11544,13 @@
         <v>8</v>
       </c>
       <c r="AK37">
-        <v>72.900000000000006</v>
+        <v>31.9</v>
       </c>
       <c r="AL37">
-        <v>6.6725199999999996</v>
+        <v>6.085</v>
       </c>
       <c r="AM37">
-        <v>1079</v>
+        <v>4831</v>
       </c>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.25">
@@ -11631,13 +11642,13 @@
         <v>8</v>
       </c>
       <c r="AK38">
-        <v>59.5</v>
+        <v>24.2</v>
       </c>
       <c r="AL38">
-        <v>7.0993599999999999</v>
+        <v>5.7175399999999996</v>
       </c>
       <c r="AM38">
-        <v>781</v>
+        <v>361</v>
       </c>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
@@ -11729,13 +11740,13 @@
         <v>8</v>
       </c>
       <c r="AK39">
-        <v>69.3</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="AL39">
-        <v>11.0715</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="AM39">
-        <v>924</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
@@ -11827,13 +11838,13 @@
         <v>8</v>
       </c>
       <c r="AK40">
-        <v>93.3</v>
+        <v>43.8</v>
       </c>
       <c r="AL40">
-        <v>8.3982799999999997</v>
+        <v>7.6003999999999996</v>
       </c>
       <c r="AM40">
-        <v>1289</v>
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
@@ -11925,13 +11936,13 @@
         <v>8</v>
       </c>
       <c r="AK41">
-        <v>57.5</v>
+        <v>23.8</v>
       </c>
       <c r="AL41">
-        <v>6.9726800000000004</v>
+        <v>5.4971800000000002</v>
       </c>
       <c r="AM41">
-        <v>897</v>
+        <v>581</v>
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
@@ -12023,13 +12034,13 @@
         <v>8</v>
       </c>
       <c r="AK42">
-        <v>82.1</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="AL42">
-        <v>9.6755099999999992</v>
+        <v>9.0327800000000007</v>
       </c>
       <c r="AM42">
-        <v>10673</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
@@ -12121,13 +12132,13 @@
         <v>8</v>
       </c>
       <c r="AK43">
-        <v>58.4</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="AL43">
-        <v>5.3610600000000002</v>
+        <v>4.2816700000000001</v>
       </c>
       <c r="AM43">
-        <v>924</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
@@ -12219,13 +12230,13 @@
         <v>8</v>
       </c>
       <c r="AK44">
-        <v>85.5</v>
+        <v>33.5</v>
       </c>
       <c r="AL44">
-        <v>7.2281300000000002</v>
+        <v>5.6983300000000003</v>
       </c>
       <c r="AM44">
-        <v>1022</v>
+        <v>448</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
@@ -12317,13 +12328,13 @@
         <v>8</v>
       </c>
       <c r="AK45">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="AL45">
-        <v>6.8568899999999999</v>
+        <v>7.4517499999999997</v>
       </c>
       <c r="AM45">
-        <v>1075</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.25">
@@ -12415,13 +12426,13 @@
         <v>8</v>
       </c>
       <c r="AK46">
-        <v>86.2</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="AL46">
-        <v>6.9162699999999999</v>
+        <v>6.2011900000000004</v>
       </c>
       <c r="AM46">
-        <v>895</v>
+        <v>435</v>
       </c>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
@@ -12513,13 +12524,13 @@
         <v>8</v>
       </c>
       <c r="AK47">
-        <v>64</v>
+        <v>20.3</v>
       </c>
       <c r="AL47">
-        <v>5.4484500000000002</v>
+        <v>4.5525399999999996</v>
       </c>
       <c r="AM47">
-        <v>783</v>
+        <v>384</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
@@ -12611,13 +12622,13 @@
         <v>8</v>
       </c>
       <c r="AK48">
-        <v>72</v>
+        <v>29.4</v>
       </c>
       <c r="AL48">
-        <v>7.9976900000000004</v>
+        <v>8.8083299999999998</v>
       </c>
       <c r="AM48">
-        <v>802</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
@@ -12709,13 +12720,13 @@
         <v>8</v>
       </c>
       <c r="AK49">
-        <v>78.5</v>
+        <v>30.6</v>
       </c>
       <c r="AL49">
-        <v>5.8617499999999998</v>
+        <v>4.9010699999999998</v>
       </c>
       <c r="AM49">
-        <v>913</v>
+        <v>537</v>
       </c>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
@@ -12807,13 +12818,13 @@
         <v>8</v>
       </c>
       <c r="AK50">
-        <v>53.2</v>
+        <v>31.7</v>
       </c>
       <c r="AL50">
-        <v>11.195600000000001</v>
+        <v>9.4648400000000006</v>
       </c>
       <c r="AM50">
-        <v>1602</v>
+        <v>450</v>
       </c>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.25">
@@ -12905,13 +12916,13 @@
         <v>8</v>
       </c>
       <c r="AK51">
-        <v>70.099999999999994</v>
+        <v>29.3</v>
       </c>
       <c r="AL51">
-        <v>6.7292800000000002</v>
+        <v>5.8238099999999999</v>
       </c>
       <c r="AM51">
-        <v>1047</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.25">
@@ -13003,13 +13014,13 @@
         <v>8</v>
       </c>
       <c r="AK52">
-        <v>90.9</v>
+        <v>34.1</v>
       </c>
       <c r="AL52">
-        <v>8.6945499999999996</v>
+        <v>5.9154799999999996</v>
       </c>
       <c r="AM52">
-        <v>23222</v>
+        <v>405</v>
       </c>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
@@ -13101,13 +13112,13 @@
         <v>8</v>
       </c>
       <c r="AK53">
-        <v>78.400000000000006</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="AL53">
-        <v>8.5318699999999996</v>
+        <v>6.7175000000000002</v>
       </c>
       <c r="AM53">
-        <v>1248</v>
+        <v>352</v>
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
@@ -13199,13 +13210,13 @@
         <v>8</v>
       </c>
       <c r="AK54">
-        <v>48.7</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="AL54">
-        <v>4.2790100000000004</v>
+        <v>4.8410700000000002</v>
       </c>
       <c r="AM54">
-        <v>887</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.25">
@@ -13297,13 +13308,13 @@
         <v>8</v>
       </c>
       <c r="AK55">
-        <v>81.7</v>
+        <v>31.8</v>
       </c>
       <c r="AL55">
-        <v>6.0329100000000002</v>
+        <v>5.3291700000000004</v>
       </c>
       <c r="AM55">
-        <v>1080</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.25">
@@ -13395,13 +13406,13 @@
         <v>8</v>
       </c>
       <c r="AK56">
-        <v>62.8</v>
+        <v>32.6</v>
       </c>
       <c r="AL56">
-        <v>8.2269600000000001</v>
+        <v>8.0314300000000003</v>
       </c>
       <c r="AM56">
-        <v>781</v>
+        <v>365</v>
       </c>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.25">
@@ -13493,13 +13504,13 @@
         <v>8</v>
       </c>
       <c r="AK57">
-        <v>56.5</v>
+        <v>29.1</v>
       </c>
       <c r="AL57">
-        <v>11.7538</v>
+        <v>9.3491700000000009</v>
       </c>
       <c r="AM57">
-        <v>949</v>
+        <v>255</v>
       </c>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.25">
@@ -13591,13 +13602,13 @@
         <v>8</v>
       </c>
       <c r="AK58">
-        <v>104.4</v>
+        <v>35.9</v>
       </c>
       <c r="AL58">
-        <v>12.1038</v>
+        <v>9.2057500000000001</v>
       </c>
       <c r="AM58">
-        <v>2916</v>
+        <v>334</v>
       </c>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
@@ -13689,13 +13700,13 @@
         <v>8</v>
       </c>
       <c r="AK59">
-        <v>88.9</v>
+        <v>23.2</v>
       </c>
       <c r="AL59">
-        <v>7.4957500000000001</v>
+        <v>5.6694399999999998</v>
       </c>
       <c r="AM59">
-        <v>17779</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
@@ -13787,13 +13798,13 @@
         <v>8</v>
       </c>
       <c r="AK60">
-        <v>74</v>
+        <v>37.5</v>
       </c>
       <c r="AL60">
-        <v>9.6051900000000003</v>
+        <v>8.5897199999999998</v>
       </c>
       <c r="AM60">
-        <v>966</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
@@ -13885,13 +13896,13 @@
         <v>8</v>
       </c>
       <c r="AK61">
-        <v>79.7</v>
+        <v>31</v>
       </c>
       <c r="AL61">
-        <v>5.5372899999999996</v>
+        <v>5.9082499999999998</v>
       </c>
       <c r="AM61">
-        <v>870</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.25">
@@ -13983,13 +13994,13 @@
         <v>8</v>
       </c>
       <c r="AK62">
-        <v>91.7</v>
+        <v>42.1</v>
       </c>
       <c r="AL62">
-        <v>7.0077800000000003</v>
+        <v>5.9469399999999997</v>
       </c>
       <c r="AM62">
-        <v>1034</v>
+        <v>477</v>
       </c>
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.25">
@@ -14081,13 +14092,13 @@
         <v>8</v>
       </c>
       <c r="AK63">
-        <v>70.3</v>
+        <v>18.3</v>
       </c>
       <c r="AL63">
-        <v>9.7489000000000008</v>
+        <v>6.5666700000000002</v>
       </c>
       <c r="AM63">
-        <v>876</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.25">
@@ -14179,13 +14190,13 @@
         <v>8</v>
       </c>
       <c r="AK64">
-        <v>78.7</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="AL64">
-        <v>6.2360699999999998</v>
+        <v>4.9028999999999998</v>
       </c>
       <c r="AM64">
-        <v>934</v>
+        <v>401</v>
       </c>
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.25">
@@ -14277,13 +14288,13 @@
         <v>8</v>
       </c>
       <c r="AK65">
-        <v>83.5</v>
+        <v>26.5</v>
       </c>
       <c r="AL65">
-        <v>7.9900700000000002</v>
+        <v>5.1776200000000001</v>
       </c>
       <c r="AM65">
-        <v>849</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.25">
@@ -14375,13 +14386,13 @@
         <v>8</v>
       </c>
       <c r="AK66">
-        <v>53.7</v>
+        <v>15</v>
       </c>
       <c r="AL66">
-        <v>9.9858799999999999</v>
+        <v>4.2708300000000001</v>
       </c>
       <c r="AM66">
-        <v>807</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:39" x14ac:dyDescent="0.25">
@@ -14473,13 +14484,13 @@
         <v>8</v>
       </c>
       <c r="AK67">
-        <v>88</v>
+        <v>27.7</v>
       </c>
       <c r="AL67">
-        <v>11.2415</v>
+        <v>7.7083300000000001</v>
       </c>
       <c r="AM67">
-        <v>1180</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:39" x14ac:dyDescent="0.25">
@@ -14571,13 +14582,13 @@
         <v>8</v>
       </c>
       <c r="AK68">
-        <v>59.7</v>
+        <v>21</v>
       </c>
       <c r="AL68">
-        <v>8.5413899999999998</v>
+        <v>6.8635700000000002</v>
       </c>
       <c r="AM68">
-        <v>15737</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:39" x14ac:dyDescent="0.25">
@@ -14669,13 +14680,13 @@
         <v>8</v>
       </c>
       <c r="AK69">
-        <v>66.099999999999994</v>
+        <v>17.8</v>
       </c>
       <c r="AL69">
-        <v>10.5395</v>
+        <v>6.75143</v>
       </c>
       <c r="AM69">
-        <v>1348</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:39" x14ac:dyDescent="0.25">
@@ -14767,13 +14778,13 @@
         <v>8</v>
       </c>
       <c r="AK70">
-        <v>51.4</v>
+        <v>23.5</v>
       </c>
       <c r="AL70">
-        <v>10.7964</v>
+        <v>5.6183300000000003</v>
       </c>
       <c r="AM70">
-        <v>757</v>
+        <v>419</v>
       </c>
     </row>
     <row r="71" spans="1:39" x14ac:dyDescent="0.25">
@@ -14865,13 +14876,13 @@
         <v>8</v>
       </c>
       <c r="AK71">
-        <v>58.6</v>
+        <v>20.7</v>
       </c>
       <c r="AL71">
-        <v>6.3501899999999996</v>
+        <v>5.7698799999999997</v>
       </c>
       <c r="AM71">
-        <v>1377</v>
+        <v>412</v>
       </c>
     </row>
     <row r="72" spans="1:39" x14ac:dyDescent="0.25">
@@ -14963,13 +14974,13 @@
         <v>8</v>
       </c>
       <c r="AK72">
-        <v>64.5</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="AL72">
-        <v>8.9309399999999997</v>
+        <v>4.9414300000000004</v>
       </c>
       <c r="AM72">
-        <v>801</v>
+        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:39" x14ac:dyDescent="0.25">
@@ -15061,13 +15072,13 @@
         <v>8</v>
       </c>
       <c r="AK73">
-        <v>95.4</v>
+        <v>28.4</v>
       </c>
       <c r="AL73">
-        <v>6.2254800000000001</v>
+        <v>6.9955600000000002</v>
       </c>
       <c r="AM73">
-        <v>1502</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" spans="1:39" x14ac:dyDescent="0.25">
@@ -15159,13 +15170,13 @@
         <v>8</v>
       </c>
       <c r="AK74">
-        <v>58.9</v>
+        <v>32.5</v>
       </c>
       <c r="AL74">
-        <v>8.8520000000000003</v>
+        <v>9.4279799999999998</v>
       </c>
       <c r="AM74">
-        <v>909</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:39" x14ac:dyDescent="0.25">
@@ -15257,13 +15268,13 @@
         <v>8</v>
       </c>
       <c r="AK75">
-        <v>56.4</v>
+        <v>34.4</v>
       </c>
       <c r="AL75">
-        <v>11.0463</v>
+        <v>6.2187299999999999</v>
       </c>
       <c r="AM75">
-        <v>1113</v>
+        <v>520</v>
       </c>
     </row>
     <row r="76" spans="1:39" x14ac:dyDescent="0.25">
@@ -15355,13 +15366,13 @@
         <v>8</v>
       </c>
       <c r="AK76">
-        <v>84.6</v>
+        <v>19.5</v>
       </c>
       <c r="AL76">
-        <v>6.9434800000000001</v>
+        <v>5.9084099999999999</v>
       </c>
       <c r="AM76">
-        <v>11664</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:39" x14ac:dyDescent="0.25">
@@ -15453,13 +15464,13 @@
         <v>8</v>
       </c>
       <c r="AK77">
-        <v>53.7</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="AL77">
-        <v>7.4385399999999997</v>
+        <v>5.7540500000000003</v>
       </c>
       <c r="AM77">
-        <v>5114</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:39" x14ac:dyDescent="0.25">
@@ -15551,13 +15562,13 @@
         <v>8</v>
       </c>
       <c r="AK78">
-        <v>72.900000000000006</v>
+        <v>40.5</v>
       </c>
       <c r="AL78">
-        <v>6.3161800000000001</v>
+        <v>5.4641700000000002</v>
       </c>
       <c r="AM78">
-        <v>941</v>
+        <v>349</v>
       </c>
     </row>
     <row r="79" spans="1:39" x14ac:dyDescent="0.25">
@@ -15649,13 +15660,13 @@
         <v>8</v>
       </c>
       <c r="AK79">
-        <v>103.2</v>
+        <v>28.1</v>
       </c>
       <c r="AL79">
-        <v>7.2251099999999999</v>
+        <v>5.3377800000000004</v>
       </c>
       <c r="AM79">
-        <v>1177</v>
+        <v>388</v>
       </c>
     </row>
     <row r="80" spans="1:39" x14ac:dyDescent="0.25">
@@ -15747,13 +15758,13 @@
         <v>8</v>
       </c>
       <c r="AK80">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="AL80">
-        <v>7.5076799999999997</v>
+        <v>8.0648800000000005</v>
       </c>
       <c r="AM80">
-        <v>1190</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:39" x14ac:dyDescent="0.25">
@@ -15845,13 +15856,13 @@
         <v>8</v>
       </c>
       <c r="AK81">
-        <v>71.3</v>
+        <v>43.7</v>
       </c>
       <c r="AL81">
-        <v>7.6157700000000004</v>
+        <v>5.6943700000000002</v>
       </c>
       <c r="AM81">
-        <v>1022</v>
+        <v>743</v>
       </c>
     </row>
     <row r="82" spans="1:39" x14ac:dyDescent="0.25">
@@ -15943,13 +15954,13 @@
         <v>8</v>
       </c>
       <c r="AK82">
-        <v>100.6</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="AL82">
-        <v>7.5739099999999997</v>
+        <v>6.6560300000000003</v>
       </c>
       <c r="AM82">
-        <v>1444</v>
+        <v>403</v>
       </c>
     </row>
     <row r="83" spans="1:39" x14ac:dyDescent="0.25">
@@ -16041,13 +16052,13 @@
         <v>8</v>
       </c>
       <c r="AK83">
-        <v>81.099999999999994</v>
+        <v>19.7</v>
       </c>
       <c r="AL83">
-        <v>8.6494700000000009</v>
+        <v>4.3283300000000002</v>
       </c>
       <c r="AM83">
-        <v>586</v>
+        <v>432</v>
       </c>
     </row>
     <row r="84" spans="1:39" x14ac:dyDescent="0.25">
@@ -16139,13 +16150,13 @@
         <v>8</v>
       </c>
       <c r="AK84">
-        <v>52.2</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="AL84">
-        <v>5.1710599999999998</v>
+        <v>4.9192099999999996</v>
       </c>
       <c r="AM84">
-        <v>1448</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:39" x14ac:dyDescent="0.25">
@@ -16237,13 +16248,13 @@
         <v>8</v>
       </c>
       <c r="AK85">
-        <v>55.5</v>
+        <v>36.1</v>
       </c>
       <c r="AL85">
-        <v>7.2497499999999997</v>
+        <v>5.9096000000000002</v>
       </c>
       <c r="AM85">
-        <v>823</v>
+        <v>649</v>
       </c>
     </row>
     <row r="86" spans="1:39" x14ac:dyDescent="0.25">
@@ -16335,13 +16346,13 @@
         <v>8</v>
       </c>
       <c r="AK86">
-        <v>91.4</v>
+        <v>28.1</v>
       </c>
       <c r="AL86">
-        <v>7.8109999999999999</v>
+        <v>6.4541700000000004</v>
       </c>
       <c r="AM86">
-        <v>1285</v>
+        <v>259</v>
       </c>
     </row>
     <row r="87" spans="1:39" x14ac:dyDescent="0.25">
@@ -16433,13 +16444,13 @@
         <v>8</v>
       </c>
       <c r="AK87">
-        <v>66.099999999999994</v>
+        <v>20.5</v>
       </c>
       <c r="AL87">
-        <v>6.5839800000000004</v>
+        <v>4.3748800000000001</v>
       </c>
       <c r="AM87">
-        <v>20014</v>
+        <v>443</v>
       </c>
     </row>
     <row r="88" spans="1:39" x14ac:dyDescent="0.25">
@@ -16531,13 +16542,13 @@
         <v>8</v>
       </c>
       <c r="AK88">
-        <v>59.2</v>
+        <v>30.4</v>
       </c>
       <c r="AL88">
-        <v>7.0901100000000001</v>
+        <v>5.4055999999999997</v>
       </c>
       <c r="AM88">
-        <v>1682</v>
+        <v>737</v>
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.25">
@@ -16629,13 +16640,13 @@
         <v>8</v>
       </c>
       <c r="AK89">
-        <v>58</v>
+        <v>18.3</v>
       </c>
       <c r="AL89">
-        <v>4.5538400000000001</v>
+        <v>5.7472200000000004</v>
       </c>
       <c r="AM89">
-        <v>1160</v>
+        <v>448</v>
       </c>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.25">
@@ -16727,13 +16738,13 @@
         <v>8</v>
       </c>
       <c r="AK90">
-        <v>43.9</v>
+        <v>20.9</v>
       </c>
       <c r="AL90">
-        <v>8.4394899999999993</v>
+        <v>4.4325000000000001</v>
       </c>
       <c r="AM90">
-        <v>951</v>
+        <v>232</v>
       </c>
     </row>
     <row r="91" spans="1:39" x14ac:dyDescent="0.25">
@@ -16825,13 +16836,13 @@
         <v>8</v>
       </c>
       <c r="AK91">
-        <v>63.6</v>
+        <v>35.9</v>
       </c>
       <c r="AL91">
-        <v>6.1083400000000001</v>
+        <v>8.1281700000000008</v>
       </c>
       <c r="AM91">
-        <v>1456</v>
+        <v>423</v>
       </c>
     </row>
     <row r="92" spans="1:39" x14ac:dyDescent="0.25">
@@ -16923,13 +16934,13 @@
         <v>8</v>
       </c>
       <c r="AK92">
-        <v>60.8</v>
+        <v>27.8</v>
       </c>
       <c r="AL92">
-        <v>7.7574800000000002</v>
+        <v>6.36972</v>
       </c>
       <c r="AM92">
-        <v>1014</v>
+        <v>252</v>
       </c>
     </row>
     <row r="93" spans="1:39" x14ac:dyDescent="0.25">
@@ -17021,13 +17032,13 @@
         <v>8</v>
       </c>
       <c r="AK93">
-        <v>84.1</v>
+        <v>35</v>
       </c>
       <c r="AL93">
-        <v>8.9840900000000001</v>
+        <v>8.0448400000000007</v>
       </c>
       <c r="AM93">
-        <v>1518</v>
+        <v>500</v>
       </c>
     </row>
     <row r="94" spans="1:39" x14ac:dyDescent="0.25">
@@ -17119,13 +17130,13 @@
         <v>8</v>
       </c>
       <c r="AK94">
-        <v>86.5</v>
+        <v>39.1</v>
       </c>
       <c r="AL94">
-        <v>10.0192</v>
+        <v>5.9371</v>
       </c>
       <c r="AM94">
-        <v>919</v>
+        <v>434</v>
       </c>
     </row>
     <row r="95" spans="1:39" x14ac:dyDescent="0.25">
@@ -17217,13 +17228,13 @@
         <v>8</v>
       </c>
       <c r="AK95">
-        <v>79.900000000000006</v>
+        <v>44.1</v>
       </c>
       <c r="AL95">
-        <v>7.8626399999999999</v>
+        <v>7.4776199999999999</v>
       </c>
       <c r="AM95">
-        <v>1459</v>
+        <v>566</v>
       </c>
     </row>
     <row r="96" spans="1:39" x14ac:dyDescent="0.25">
@@ -17315,13 +17326,13 @@
         <v>8</v>
       </c>
       <c r="AK96">
-        <v>78.3</v>
+        <v>31.2</v>
       </c>
       <c r="AL96">
-        <v>6.6682800000000002</v>
+        <v>5.7110300000000001</v>
       </c>
       <c r="AM96">
-        <v>1827</v>
+        <v>349</v>
       </c>
     </row>
     <row r="97" spans="1:39" x14ac:dyDescent="0.25">
@@ -17413,13 +17424,13 @@
         <v>8</v>
       </c>
       <c r="AK97">
-        <v>76.599999999999994</v>
+        <v>26.3</v>
       </c>
       <c r="AL97">
-        <v>7.9331300000000002</v>
+        <v>6.28024</v>
       </c>
       <c r="AM97">
-        <v>1637</v>
+        <v>457</v>
       </c>
     </row>
     <row r="98" spans="1:39" x14ac:dyDescent="0.25">
@@ -17511,13 +17522,13 @@
         <v>8</v>
       </c>
       <c r="AK98">
-        <v>62.7</v>
+        <v>30.2</v>
       </c>
       <c r="AL98">
-        <v>6.8227900000000004</v>
+        <v>9.0514299999999999</v>
       </c>
       <c r="AM98">
-        <v>3045</v>
+        <v>229</v>
       </c>
     </row>
     <row r="99" spans="1:39" x14ac:dyDescent="0.25">
@@ -17609,13 +17620,13 @@
         <v>8</v>
       </c>
       <c r="AK99">
-        <v>68.900000000000006</v>
+        <v>22.2</v>
       </c>
       <c r="AL99">
-        <v>10.9648</v>
+        <v>4.7957099999999997</v>
       </c>
       <c r="AM99">
-        <v>1473</v>
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:39" x14ac:dyDescent="0.25">
@@ -17707,13 +17718,13 @@
         <v>8</v>
       </c>
       <c r="AK100">
-        <v>79.900000000000006</v>
+        <v>20.5</v>
       </c>
       <c r="AL100">
-        <v>7.8626399999999999</v>
+        <v>4.3748800000000001</v>
       </c>
       <c r="AM100">
-        <v>1459</v>
+        <v>443</v>
       </c>
     </row>
     <row r="101" spans="1:39" x14ac:dyDescent="0.25">
@@ -17805,13 +17816,13 @@
         <v>8</v>
       </c>
       <c r="AK101">
-        <v>78.3</v>
+        <v>30.4</v>
       </c>
       <c r="AL101">
-        <v>6.6682800000000002</v>
+        <v>5.4055999999999997</v>
       </c>
       <c r="AM101">
-        <v>1827</v>
+        <v>737</v>
       </c>
     </row>
     <row r="102" spans="1:39" x14ac:dyDescent="0.25">
@@ -17867,13 +17878,142 @@
         <v>8</v>
       </c>
       <c r="AK102">
-        <v>76.599999999999994</v>
+        <v>18.3</v>
       </c>
       <c r="AL102">
-        <v>7.9331300000000002</v>
+        <v>5.7472200000000004</v>
       </c>
       <c r="AM102">
-        <v>1637</v>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="103" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <f>AVERAGE(B2:B102)</f>
+        <v>31.36099999999999</v>
+      </c>
+      <c r="C103">
+        <f t="shared" ref="C103:AM103" si="0">AVERAGE(C2:C102)</f>
+        <v>6.6822836000000025</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="0"/>
+        <v>395.01</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="0"/>
+        <v>20.302999999999997</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="0"/>
+        <v>3.2288945999999985</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="0"/>
+        <v>462.15</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="0"/>
+        <v>19.934000000000001</v>
+      </c>
+      <c r="M103">
+        <f t="shared" si="0"/>
+        <v>2.9206245000000006</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="0"/>
+        <v>474.39</v>
+      </c>
+      <c r="P103">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q103">
+        <f t="shared" si="0"/>
+        <v>21.64950495049505</v>
+      </c>
+      <c r="R103">
+        <f t="shared" si="0"/>
+        <v>3.9467704950495017</v>
+      </c>
+      <c r="S103">
+        <f t="shared" si="0"/>
+        <v>312.70297029702971</v>
+      </c>
+      <c r="U103">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="V103">
+        <f t="shared" si="0"/>
+        <v>21.922772277227708</v>
+      </c>
+      <c r="W103">
+        <f t="shared" si="0"/>
+        <v>4.009032277227722</v>
+      </c>
+      <c r="X103">
+        <f t="shared" si="0"/>
+        <v>384.14851485148517</v>
+      </c>
+      <c r="Z103">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AA103">
+        <f t="shared" si="0"/>
+        <v>26.063366336633681</v>
+      </c>
+      <c r="AB103">
+        <f t="shared" si="0"/>
+        <v>6.9349315841584112</v>
+      </c>
+      <c r="AC103">
+        <f t="shared" si="0"/>
+        <v>440.83168316831683</v>
+      </c>
+      <c r="AE103">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AF103">
+        <f t="shared" si="0"/>
+        <v>27.324752475247536</v>
+      </c>
+      <c r="AG103">
+        <f t="shared" si="0"/>
+        <v>6.8019806930693072</v>
+      </c>
+      <c r="AH103">
+        <f t="shared" si="0"/>
+        <v>377.28712871287127</v>
+      </c>
+      <c r="AJ103">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AK103">
+        <f t="shared" si="0"/>
+        <v>30.687128712871274</v>
+      </c>
+      <c r="AL103">
+        <f t="shared" si="0"/>
+        <v>6.5794434653465341</v>
+      </c>
+      <c r="AM103">
+        <f t="shared" si="0"/>
+        <v>448.21782178217819</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tests ran on external priority algorithms
</commit_message>
<xml_diff>
--- a/ProcessSimulator/N=10 Graphs.xlsx
+++ b/ProcessSimulator/N=10 Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\MST\Fall 2020\CS 3800\Project\Simulator\Process-Memory-Mangaement-Simulation\ProcessSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80C7477-824E-4AFD-BA0C-F278386A0C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2097F6-3945-498C-8750-73B25B45119F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="690" yWindow="7185" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3333,7 +3333,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Time for All 100 Process (n) Lists on All Algorithms Where n=10 </a:t>
+              <a:t> Time for All 100 Process (n) Lists on All Algorithms Where n=10 and Small Execution Time </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -6417,7 +6417,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7921,8 +7921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L58" workbookViewId="0">
-      <selection activeCell="AM103" sqref="AM103"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="X167" sqref="X167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>